<commit_message>
Data importation and start of main code
</commit_message>
<xml_diff>
--- a/Data/Cleaned data/Andamento mensile per settore (Cinema).xlsx
+++ b/Data/Cleaned data/Andamento mensile per settore (Cinema).xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/albertocalabrese99/Desktop/Statistical learning/Statistical_Learning_Project/Data/Cleaned data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9D5EE5-111F-924C-81B1-863E48CB3E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3129F3FF-2767-D54A-AF5C-E92A35895A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Numero spettacoli" sheetId="2" r:id="rId1"/>
     <sheet name="Ingressi" sheetId="3" r:id="rId2"/>
     <sheet name="Spesa del pubblico" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="17">
   <si>
     <t>Mese evento</t>
   </si>
@@ -67,6 +68,18 @@
   <si>
     <t>Dicembre</t>
   </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Numero spettacoli</t>
+  </si>
+  <si>
+    <t>Ingressi</t>
+  </si>
+  <si>
+    <t>Spesa del pubblico</t>
+  </si>
 </sst>
 </file>
 
@@ -101,8 +114,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,7 +409,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B2" sqref="B2:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -652,7 +666,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F13"/>
+      <selection activeCell="B2" sqref="B2:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -905,8 +919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3080E2F2-3342-47B6-9B25-7CD120F31868}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1177,4 +1191,831 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71519923-B505-8D4B-962B-6A4BB378CC6A}">
+  <dimension ref="A1:D61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>43101</v>
+      </c>
+      <c r="B2">
+        <v>319556</v>
+      </c>
+      <c r="C2">
+        <v>12815316</v>
+      </c>
+      <c r="D2">
+        <v>99527809.399999902</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>43132</v>
+      </c>
+      <c r="B3">
+        <v>279211</v>
+      </c>
+      <c r="C3">
+        <v>10586422</v>
+      </c>
+      <c r="D3">
+        <v>78156505.449999973</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>43160</v>
+      </c>
+      <c r="B4">
+        <v>302038</v>
+      </c>
+      <c r="C4">
+        <v>8408634</v>
+      </c>
+      <c r="D4">
+        <v>60683989.140000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>43191</v>
+      </c>
+      <c r="B5">
+        <v>287672</v>
+      </c>
+      <c r="C5">
+        <v>7429757</v>
+      </c>
+      <c r="D5">
+        <v>52284212.710000023</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>43221</v>
+      </c>
+      <c r="B6">
+        <v>262643</v>
+      </c>
+      <c r="C6">
+        <v>5579501</v>
+      </c>
+      <c r="D6">
+        <v>45098825.430000059</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>43252</v>
+      </c>
+      <c r="B7">
+        <v>212699</v>
+      </c>
+      <c r="C7">
+        <v>3675420</v>
+      </c>
+      <c r="D7">
+        <v>28124127.300000008</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>43282</v>
+      </c>
+      <c r="B8">
+        <v>176592</v>
+      </c>
+      <c r="C8">
+        <v>2972751</v>
+      </c>
+      <c r="D8">
+        <v>19073912.039999984</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>43313</v>
+      </c>
+      <c r="B9">
+        <v>187101</v>
+      </c>
+      <c r="C9">
+        <v>5110096</v>
+      </c>
+      <c r="D9">
+        <v>37118997.81000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>43344</v>
+      </c>
+      <c r="B10">
+        <v>264158</v>
+      </c>
+      <c r="C10">
+        <v>6789039</v>
+      </c>
+      <c r="D10">
+        <v>52631424.299999967</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>43374</v>
+      </c>
+      <c r="B11">
+        <v>281824</v>
+      </c>
+      <c r="C11">
+        <v>7709847</v>
+      </c>
+      <c r="D11">
+        <v>57354454.720000006</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>43405</v>
+      </c>
+      <c r="B12">
+        <v>279071</v>
+      </c>
+      <c r="C12">
+        <v>8672730</v>
+      </c>
+      <c r="D12">
+        <v>62379808.1599999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>43435</v>
+      </c>
+      <c r="B13">
+        <v>312125</v>
+      </c>
+      <c r="C13">
+        <v>11938186</v>
+      </c>
+      <c r="D13">
+        <v>89976686.61999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>43466</v>
+      </c>
+      <c r="B14">
+        <v>308748</v>
+      </c>
+      <c r="C14">
+        <v>12489100</v>
+      </c>
+      <c r="D14">
+        <v>100171903.29999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>43497</v>
+      </c>
+      <c r="B15">
+        <v>272951</v>
+      </c>
+      <c r="C15">
+        <v>8467518</v>
+      </c>
+      <c r="D15">
+        <v>61659419.879999988</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>43525</v>
+      </c>
+      <c r="B16">
+        <v>301053</v>
+      </c>
+      <c r="C16">
+        <v>8068654</v>
+      </c>
+      <c r="D16">
+        <v>59014191.740000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>43556</v>
+      </c>
+      <c r="B17">
+        <v>288046</v>
+      </c>
+      <c r="C17">
+        <v>10290518</v>
+      </c>
+      <c r="D17">
+        <v>77990289.280000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>43586</v>
+      </c>
+      <c r="B18">
+        <v>268636</v>
+      </c>
+      <c r="C18">
+        <v>7796085</v>
+      </c>
+      <c r="D18">
+        <v>59729552.510000013</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>43617</v>
+      </c>
+      <c r="B19">
+        <v>237477</v>
+      </c>
+      <c r="C19">
+        <v>4286370</v>
+      </c>
+      <c r="D19">
+        <v>31849329.549999993</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>43647</v>
+      </c>
+      <c r="B20">
+        <v>207763</v>
+      </c>
+      <c r="C20">
+        <v>4909151</v>
+      </c>
+      <c r="D20">
+        <v>37861308.359999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>43678</v>
+      </c>
+      <c r="B21">
+        <v>210585</v>
+      </c>
+      <c r="C21">
+        <v>7051071</v>
+      </c>
+      <c r="D21">
+        <v>54350700.960000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>43709</v>
+      </c>
+      <c r="B22">
+        <v>252819</v>
+      </c>
+      <c r="C22">
+        <v>7819079</v>
+      </c>
+      <c r="D22">
+        <v>62794563.509999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>43739</v>
+      </c>
+      <c r="B23">
+        <v>284646</v>
+      </c>
+      <c r="C23">
+        <v>9632400</v>
+      </c>
+      <c r="D23">
+        <v>72910605.820000008</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>43770</v>
+      </c>
+      <c r="B24">
+        <v>291507</v>
+      </c>
+      <c r="C24">
+        <v>9937379</v>
+      </c>
+      <c r="D24">
+        <v>70529036.690000027</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>43800</v>
+      </c>
+      <c r="B25">
+        <v>321114</v>
+      </c>
+      <c r="C25">
+        <v>13691888</v>
+      </c>
+      <c r="D25">
+        <v>103129044.45999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>43831</v>
+      </c>
+      <c r="B26">
+        <v>342511</v>
+      </c>
+      <c r="C26">
+        <v>16606889</v>
+      </c>
+      <c r="D26">
+        <v>121440619.01000008</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>43862</v>
+      </c>
+      <c r="B27">
+        <v>251640</v>
+      </c>
+      <c r="C27">
+        <v>7080523</v>
+      </c>
+      <c r="D27">
+        <v>48923544.429999985</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>43891</v>
+      </c>
+      <c r="B28">
+        <v>14247</v>
+      </c>
+      <c r="C28">
+        <v>217518</v>
+      </c>
+      <c r="D28">
+        <v>1440488.9799999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>43922</v>
+      </c>
+      <c r="D29">
+        <v>325.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>43952</v>
+      </c>
+      <c r="D30">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>43983</v>
+      </c>
+      <c r="B31">
+        <v>6944</v>
+      </c>
+      <c r="C31">
+        <v>111677</v>
+      </c>
+      <c r="D31">
+        <v>685211.22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>44013</v>
+      </c>
+      <c r="B32">
+        <v>23934</v>
+      </c>
+      <c r="C32">
+        <v>658929</v>
+      </c>
+      <c r="D32">
+        <v>3309540.71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>44044</v>
+      </c>
+      <c r="B33">
+        <v>59427</v>
+      </c>
+      <c r="C33">
+        <v>1381564</v>
+      </c>
+      <c r="D33">
+        <v>7665196.5400000019</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>44075</v>
+      </c>
+      <c r="B34">
+        <v>158221</v>
+      </c>
+      <c r="C34">
+        <v>2443035</v>
+      </c>
+      <c r="D34">
+        <v>17362260.849999994</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>44105</v>
+      </c>
+      <c r="B35">
+        <v>139085</v>
+      </c>
+      <c r="C35">
+        <v>1805636</v>
+      </c>
+      <c r="D35">
+        <v>11266608.920000006</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>44136</v>
+      </c>
+      <c r="D36">
+        <v>4823.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>44166</v>
+      </c>
+      <c r="D37">
+        <v>56332</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>44197</v>
+      </c>
+      <c r="D38">
+        <v>27483</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>44228</v>
+      </c>
+      <c r="D39">
+        <v>14353.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>44256</v>
+      </c>
+      <c r="D40">
+        <v>2164.8000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>44287</v>
+      </c>
+      <c r="B41">
+        <v>2174</v>
+      </c>
+      <c r="C41">
+        <v>44478</v>
+      </c>
+      <c r="D41">
+        <v>289498.68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>44317</v>
+      </c>
+      <c r="B42">
+        <v>61019</v>
+      </c>
+      <c r="C42">
+        <v>801049</v>
+      </c>
+      <c r="D42">
+        <v>5164938.1400000006</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>44348</v>
+      </c>
+      <c r="B43">
+        <v>124073</v>
+      </c>
+      <c r="C43">
+        <v>1415528</v>
+      </c>
+      <c r="D43">
+        <v>9102229.3499999996</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>44378</v>
+      </c>
+      <c r="B44">
+        <v>137767</v>
+      </c>
+      <c r="C44">
+        <v>2318804</v>
+      </c>
+      <c r="D44">
+        <v>15407893.210000005</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>44409</v>
+      </c>
+      <c r="B45">
+        <v>156915</v>
+      </c>
+      <c r="C45">
+        <v>2679886</v>
+      </c>
+      <c r="D45">
+        <v>18074571.25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>44440</v>
+      </c>
+      <c r="B46">
+        <v>187832</v>
+      </c>
+      <c r="C46">
+        <v>3272931</v>
+      </c>
+      <c r="D46">
+        <v>22875671.269999988</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>44470</v>
+      </c>
+      <c r="B47">
+        <v>217862</v>
+      </c>
+      <c r="C47">
+        <v>5048158</v>
+      </c>
+      <c r="D47">
+        <v>35585479.210000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>44501</v>
+      </c>
+      <c r="B48">
+        <v>225776</v>
+      </c>
+      <c r="C48">
+        <v>5050651</v>
+      </c>
+      <c r="D48">
+        <v>34525123.079999991</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>44531</v>
+      </c>
+      <c r="B49">
+        <v>237348</v>
+      </c>
+      <c r="C49">
+        <v>6101141</v>
+      </c>
+      <c r="D49">
+        <v>44847154.659999996</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>44562</v>
+      </c>
+      <c r="B50">
+        <v>250091</v>
+      </c>
+      <c r="C50">
+        <v>4536594</v>
+      </c>
+      <c r="D50">
+        <v>32381225.899999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>44593</v>
+      </c>
+      <c r="B51">
+        <v>170035</v>
+      </c>
+      <c r="C51">
+        <v>2978630</v>
+      </c>
+      <c r="D51">
+        <v>20299393.849999998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B52">
+        <v>199764</v>
+      </c>
+      <c r="C52">
+        <v>3658086</v>
+      </c>
+      <c r="D52">
+        <v>24659053.099999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>44652</v>
+      </c>
+      <c r="B53">
+        <v>212027</v>
+      </c>
+      <c r="C53">
+        <v>4048463</v>
+      </c>
+      <c r="D53">
+        <v>27809817.410000008</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>44682</v>
+      </c>
+      <c r="B54">
+        <v>187349</v>
+      </c>
+      <c r="C54">
+        <v>3792309</v>
+      </c>
+      <c r="D54">
+        <v>27234239.390000012</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>44713</v>
+      </c>
+      <c r="B55">
+        <v>159464</v>
+      </c>
+      <c r="C55">
+        <v>3065783</v>
+      </c>
+      <c r="D55">
+        <v>21926129.690000009</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>44743</v>
+      </c>
+      <c r="B56">
+        <v>125896</v>
+      </c>
+      <c r="C56">
+        <v>2687118</v>
+      </c>
+      <c r="D56">
+        <v>18478583.930000003</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>44774</v>
+      </c>
+      <c r="B57">
+        <v>126277</v>
+      </c>
+      <c r="C57">
+        <v>3036152</v>
+      </c>
+      <c r="D57">
+        <v>20729046.200000003</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>44805</v>
+      </c>
+      <c r="B58">
+        <v>178988</v>
+      </c>
+      <c r="C58">
+        <v>3667427</v>
+      </c>
+      <c r="D58">
+        <v>22258833.90000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>44835</v>
+      </c>
+      <c r="B59">
+        <v>211458</v>
+      </c>
+      <c r="C59">
+        <v>4364739</v>
+      </c>
+      <c r="D59">
+        <v>30259469.300000016</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>44866</v>
+      </c>
+      <c r="B60">
+        <v>208221</v>
+      </c>
+      <c r="C60">
+        <v>4946407</v>
+      </c>
+      <c r="D60">
+        <v>33332163.960000012</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>44896</v>
+      </c>
+      <c r="B61">
+        <v>225459</v>
+      </c>
+      <c r="C61">
+        <v>6869912</v>
+      </c>
+      <c r="D61">
+        <v>53667485.470000006</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>